<commit_message>
Actualizacion README - Indicacion Ruta de Script
</commit_message>
<xml_diff>
--- a/examples/TEST_FILE_VR_201_221_.xlsx
+++ b/examples/TEST_FILE_VR_201_221_.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kher-\proyectos\sap_scripts_generator\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2153B8D-9BCE-43BF-8BA7-EB037C3CF7CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3361E94E-2535-460C-8332-369A970CB0B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="40">
   <si>
     <t>PO</t>
   </si>
@@ -159,6 +159,9 @@
   </si>
   <si>
     <t>MOV_SAP</t>
+  </si>
+  <si>
+    <t>ATENDIDO</t>
   </si>
 </sst>
 </file>
@@ -572,10 +575,10 @@
   <dimension ref="A1:Q12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K17" sqref="K17"/>
+      <selection pane="bottomRight" activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -907,7 +910,7 @@
         <v>3</v>
       </c>
       <c r="Q6" s="11" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
@@ -959,7 +962,7 @@
         <v>3</v>
       </c>
       <c r="Q7" s="11" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
@@ -1011,7 +1014,7 @@
         <v>3</v>
       </c>
       <c r="Q8" s="11" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
@@ -1063,7 +1066,7 @@
         <v>4</v>
       </c>
       <c r="Q9" s="11" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
@@ -1115,7 +1118,7 @@
         <v>4</v>
       </c>
       <c r="Q10" s="11" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
@@ -1167,7 +1170,7 @@
         <v>4</v>
       </c>
       <c r="Q11" s="11" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
@@ -1219,7 +1222,7 @@
         <v>4</v>
       </c>
       <c r="Q12" s="11" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>